<commit_message>
Write numbers as numbers
</commit_message>
<xml_diff>
--- a/test/files/example.xlsx
+++ b/test/files/example.xlsx
@@ -380,7 +380,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10"/>
+    <row r="2" spans="1:10">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+    </row>
     <row r="3" spans="1:10"/>
     <row r="4" spans="1:10"/>
     <row r="5" spans="1:10"/>

</xml_diff>

<commit_message>
Update tests to reflect named ranges; bump package version
</commit_message>
<xml_diff>
--- a/test/files/example.xlsx
+++ b/test/files/example.xlsx
@@ -9,9 +9,7 @@
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" hidden="1" localSheetId="0">'sheet1'!$A$1:$J$12</definedName>
-  </definedNames>
+  <definedNames/>
   <calcPr calcId="124519"/>
 </workbook>
 </file>

</xml_diff>

<commit_message>
Update to add notes
</commit_message>
<xml_diff>
--- a/test/files/example.xlsx
+++ b/test/files/example.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
@@ -15,24 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>I am title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -40,7 +23,7 @@
   <fonts count="1">
     <font>
       <sz val="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -72,10 +55,10 @@
     </xf>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -369,167 +352,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="7" state="frozen" activePane="bottomRight" topLeftCell="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1">
         <v>1</v>
       </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
       <c r="C1" t="s">
+        <v>-1</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2"/>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>4</v>
       </c>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
+      <c r="C3">
+        <v>NaN</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>